<commit_message>
working on grasp documentation
</commit_message>
<xml_diff>
--- a/hw2_GRASP/Results.xlsx
+++ b/hw2_GRASP/Results.xlsx
@@ -8,14 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saleh\Desktop\Master\semester 2\advanced algorithms\Hws\hw2_GRASP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D681EC53-0130-4D7F-AFBE-B43A0B1D3ED1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00418A6-499B-4307-A349-05D261D694F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3552" yWindow="1800" windowWidth="14436" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -704,7 +712,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-3000401]#,##0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -748,6 +756,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -769,7 +785,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -803,6 +819,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1083,10 +1100,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K60"/>
+  <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1132,7 +1149,9 @@
       <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="2">
+        <v>41</v>
+      </c>
       <c r="C2" s="1"/>
       <c r="D2" s="9">
         <v>61</v>
@@ -1153,12 +1172,18 @@
         <v>4</v>
       </c>
       <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
+      <c r="K2" s="9">
+        <f>D2-B2</f>
+        <v>20</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>6</v>
       </c>
+      <c r="B3" s="2">
+        <v>55</v>
+      </c>
       <c r="D3">
         <v>63</v>
       </c>
@@ -1176,12 +1201,19 @@
       </c>
       <c r="I3" t="s">
         <v>9</v>
+      </c>
+      <c r="K3" s="9">
+        <f t="shared" ref="K3:K55" si="0">D3-B3</f>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
+      <c r="B4" s="2">
+        <v>55</v>
+      </c>
       <c r="D4">
         <v>63</v>
       </c>
@@ -1199,12 +1231,19 @@
       </c>
       <c r="I4" t="s">
         <v>13</v>
+      </c>
+      <c r="K4" s="9">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
+      <c r="B5" s="2">
+        <v>18230</v>
+      </c>
       <c r="D5">
         <v>20635</v>
       </c>
@@ -1222,12 +1261,19 @@
       </c>
       <c r="I5" t="s">
         <v>17</v>
+      </c>
+      <c r="K5" s="9">
+        <f t="shared" si="0"/>
+        <v>2405</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
+      <c r="B6" s="2">
+        <v>2125</v>
+      </c>
       <c r="D6">
         <v>2125</v>
       </c>
@@ -1245,12 +1291,19 @@
       </c>
       <c r="I6" t="s">
         <v>21</v>
+      </c>
+      <c r="K6" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
+      <c r="B7" s="2">
+        <v>8026</v>
+      </c>
       <c r="D7">
         <v>11116</v>
       </c>
@@ -1268,12 +1321,19 @@
       </c>
       <c r="I7" t="s">
         <v>25</v>
+      </c>
+      <c r="K7" s="9">
+        <f t="shared" si="0"/>
+        <v>3090</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>26</v>
       </c>
+      <c r="B8" s="2">
+        <v>40419</v>
+      </c>
       <c r="D8">
         <v>45107</v>
       </c>
@@ -1291,12 +1351,19 @@
       </c>
       <c r="I8" t="s">
         <v>29</v>
+      </c>
+      <c r="K8" s="9">
+        <f t="shared" si="0"/>
+        <v>4688</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>30</v>
       </c>
+      <c r="B9" s="2">
+        <v>39420</v>
+      </c>
       <c r="D9">
         <v>48730</v>
       </c>
@@ -1314,12 +1381,19 @@
       </c>
       <c r="I9" t="s">
         <v>33</v>
+      </c>
+      <c r="K9" s="9">
+        <f t="shared" si="0"/>
+        <v>9310</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>34</v>
       </c>
+      <c r="B10" s="2">
+        <v>49499</v>
+      </c>
       <c r="D10">
         <v>61675</v>
       </c>
@@ -1337,12 +1411,19 @@
       </c>
       <c r="I10" t="s">
         <v>37</v>
+      </c>
+      <c r="K10" s="9">
+        <f t="shared" si="0"/>
+        <v>12176</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>38</v>
       </c>
+      <c r="B11" s="2">
+        <v>28140</v>
+      </c>
       <c r="D11">
         <v>29120</v>
       </c>
@@ -1360,12 +1441,19 @@
       </c>
       <c r="I11" t="s">
         <v>41</v>
+      </c>
+      <c r="K11" s="9">
+        <f t="shared" si="0"/>
+        <v>980</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>42</v>
       </c>
+      <c r="B12" s="2">
+        <v>83005</v>
+      </c>
       <c r="D12">
         <v>84820</v>
       </c>
@@ -1383,12 +1471,19 @@
       </c>
       <c r="I12" t="s">
         <v>45</v>
+      </c>
+      <c r="K12" s="9">
+        <f t="shared" si="0"/>
+        <v>1815</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>46</v>
       </c>
+      <c r="B13" s="2">
+        <v>1123</v>
+      </c>
       <c r="D13">
         <v>2062</v>
       </c>
@@ -1406,12 +1501,19 @@
       </c>
       <c r="I13" t="s">
         <v>49</v>
+      </c>
+      <c r="K13" s="9">
+        <f t="shared" si="0"/>
+        <v>939</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>50</v>
       </c>
+      <c r="B14" s="2">
+        <v>243</v>
+      </c>
       <c r="D14">
         <v>417</v>
       </c>
@@ -1429,12 +1531,19 @@
       </c>
       <c r="I14" t="s">
         <v>53</v>
+      </c>
+      <c r="K14" s="9">
+        <f t="shared" si="0"/>
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>54</v>
       </c>
+      <c r="B15" s="2">
+        <v>1071</v>
+      </c>
       <c r="D15">
         <v>2477</v>
       </c>
@@ -1452,12 +1561,19 @@
       </c>
       <c r="I15" t="s">
         <v>57</v>
+      </c>
+      <c r="K15" s="9">
+        <f t="shared" si="0"/>
+        <v>1406</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>58</v>
       </c>
+      <c r="B16" s="2">
+        <v>912</v>
+      </c>
       <c r="D16">
         <v>1530</v>
       </c>
@@ -1476,11 +1592,18 @@
       <c r="I16" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K16" s="9">
+        <f t="shared" si="0"/>
+        <v>618</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>62</v>
       </c>
+      <c r="B17" s="2">
+        <v>915</v>
+      </c>
       <c r="D17">
         <v>1560</v>
       </c>
@@ -1499,11 +1622,18 @@
       <c r="I17" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K17" s="9">
+        <f t="shared" si="0"/>
+        <v>645</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>66</v>
       </c>
+      <c r="B18" s="2">
+        <v>879</v>
+      </c>
       <c r="D18">
         <v>1608</v>
       </c>
@@ -1522,11 +1652,18 @@
       <c r="I18" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K18" s="9">
+        <f t="shared" si="0"/>
+        <v>729</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>70</v>
       </c>
+      <c r="B19" s="2">
+        <v>400</v>
+      </c>
       <c r="D19">
         <v>474</v>
       </c>
@@ -1545,11 +1682,18 @@
       <c r="I19" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K19" s="9">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>74</v>
       </c>
+      <c r="B20" s="2">
+        <v>397</v>
+      </c>
       <c r="D20">
         <v>501</v>
       </c>
@@ -1568,11 +1712,18 @@
       <c r="I20" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K20" s="9">
+        <f t="shared" si="0"/>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>78</v>
       </c>
+      <c r="B21" s="2">
+        <v>467</v>
+      </c>
       <c r="D21">
         <v>543</v>
       </c>
@@ -1591,11 +1742,18 @@
       <c r="I21" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K21" s="9">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>82</v>
       </c>
+      <c r="B22" s="2">
+        <v>1023</v>
+      </c>
       <c r="D22">
         <v>1300</v>
       </c>
@@ -1614,11 +1772,18 @@
       <c r="I22" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K22" s="9">
+        <f t="shared" si="0"/>
+        <v>277</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>86</v>
       </c>
+      <c r="B23" s="2">
+        <v>198</v>
+      </c>
       <c r="D23">
         <v>1323</v>
       </c>
@@ -1637,11 +1802,18 @@
       <c r="I23" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K23" s="9">
+        <f t="shared" si="0"/>
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>90</v>
       </c>
+      <c r="B24" s="2">
+        <v>1494</v>
+      </c>
       <c r="D24">
         <v>1654</v>
       </c>
@@ -1660,11 +1832,18 @@
       <c r="I24" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K24" s="9">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>94</v>
       </c>
+      <c r="B25" s="2">
+        <v>1423</v>
+      </c>
       <c r="D25">
         <v>1641</v>
       </c>
@@ -1683,11 +1862,18 @@
       <c r="I25" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K25" s="9">
+        <f t="shared" si="0"/>
+        <v>218</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>98</v>
       </c>
+      <c r="B26" s="2">
+        <v>1361</v>
+      </c>
       <c r="D26">
         <v>1623</v>
       </c>
@@ -1706,11 +1892,18 @@
       <c r="I26" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K26" s="9">
+        <f t="shared" si="0"/>
+        <v>262</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>102</v>
       </c>
+      <c r="B27" s="2">
+        <v>1381</v>
+      </c>
       <c r="D27">
         <v>1678</v>
       </c>
@@ -1729,11 +1922,18 @@
       <c r="I27" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K27" s="9">
+        <f t="shared" si="0"/>
+        <v>297</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>106</v>
       </c>
+      <c r="B28" s="2">
+        <v>1765</v>
+      </c>
       <c r="D28">
         <v>2077</v>
       </c>
@@ -1752,11 +1952,18 @@
       <c r="I28" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K28" s="9">
+        <f t="shared" si="0"/>
+        <v>312</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>110</v>
       </c>
+      <c r="B29" s="2">
+        <v>1750</v>
+      </c>
       <c r="D29">
         <v>2101</v>
       </c>
@@ -1775,11 +1982,18 @@
       <c r="I29" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K29" s="9">
+        <f t="shared" si="0"/>
+        <v>351</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>114</v>
       </c>
+      <c r="B30" s="2">
+        <v>2033</v>
+      </c>
       <c r="D30">
         <v>2461</v>
       </c>
@@ -1798,11 +2012,18 @@
       <c r="I30" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K30" s="9">
+        <f t="shared" si="0"/>
+        <v>428</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>118</v>
       </c>
+      <c r="B31" s="2">
+        <v>2241</v>
+      </c>
       <c r="D31">
         <v>2826</v>
       </c>
@@ -1821,11 +2042,18 @@
       <c r="I31" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K31" s="9">
+        <f t="shared" si="0"/>
+        <v>585</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>122</v>
       </c>
+      <c r="B32" s="2">
+        <v>2544</v>
+      </c>
       <c r="D32">
         <v>3301</v>
       </c>
@@ -1844,11 +2072,18 @@
       <c r="I32" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K32" s="9">
+        <f t="shared" si="0"/>
+        <v>757</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>126</v>
       </c>
+      <c r="B33" s="2">
+        <v>3062</v>
+      </c>
       <c r="D33">
         <v>3930</v>
       </c>
@@ -1867,11 +2102,18 @@
       <c r="I33" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K33" s="9">
+        <f t="shared" si="0"/>
+        <v>868</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>130</v>
       </c>
+      <c r="B34" s="2">
+        <v>3482</v>
+      </c>
       <c r="D34">
         <v>4576</v>
       </c>
@@ -1890,11 +2132,18 @@
       <c r="I34" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K34" s="9">
+        <f t="shared" si="0"/>
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>134</v>
       </c>
+      <c r="B35" s="2">
+        <v>2568</v>
+      </c>
       <c r="D35">
         <v>4583</v>
       </c>
@@ -1913,11 +2162,18 @@
       <c r="I35" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K35" s="9">
+        <f t="shared" si="0"/>
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>138</v>
       </c>
+      <c r="B36" s="2">
+        <v>2545</v>
+      </c>
       <c r="D36">
         <v>4746</v>
       </c>
@@ -1936,11 +2192,18 @@
       <c r="I36" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K36" s="9">
+        <f t="shared" si="0"/>
+        <v>2201</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>142</v>
       </c>
+      <c r="B37" s="2">
+        <v>16666</v>
+      </c>
       <c r="D37">
         <v>20407</v>
       </c>
@@ -1959,11 +2222,18 @@
       <c r="I37" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K37" s="9">
+        <f t="shared" si="0"/>
+        <v>3741</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>146</v>
       </c>
+      <c r="B38" s="2">
+        <v>19894</v>
+      </c>
       <c r="D38">
         <v>26118</v>
       </c>
@@ -1982,410 +2252,530 @@
       <c r="I38" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K38" s="9">
+        <f t="shared" si="0"/>
+        <v>6224</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B39" s="2">
+        <v>1109</v>
+      </c>
+      <c r="D39">
+        <v>1177</v>
+      </c>
+      <c r="E39">
+        <v>1185</v>
+      </c>
+      <c r="F39">
+        <v>1194</v>
+      </c>
+      <c r="G39" t="s">
+        <v>151</v>
+      </c>
+      <c r="H39" t="s">
+        <v>152</v>
+      </c>
+      <c r="I39" t="s">
+        <v>153</v>
+      </c>
+      <c r="K39" s="9">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>150</v>
+        <v>154</v>
+      </c>
+      <c r="B40" s="2">
+        <v>577</v>
       </c>
       <c r="D40">
-        <v>1177</v>
+        <v>585</v>
       </c>
       <c r="E40">
-        <v>1185</v>
+        <v>586.4</v>
       </c>
       <c r="F40">
-        <v>1194</v>
+        <v>587</v>
       </c>
       <c r="G40" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="H40" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="I40" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+      <c r="K40" s="9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>154</v>
+        <v>158</v>
+      </c>
+      <c r="B41" s="2">
+        <v>791</v>
       </c>
       <c r="D41">
-        <v>585</v>
+        <v>856</v>
       </c>
       <c r="E41">
-        <v>586.4</v>
+        <v>865.2</v>
       </c>
       <c r="F41">
-        <v>587</v>
+        <v>875</v>
       </c>
       <c r="G41" t="s">
+        <v>159</v>
+      </c>
+      <c r="H41" t="s">
+        <v>160</v>
+      </c>
+      <c r="I41" t="s">
+        <v>161</v>
+      </c>
+      <c r="K41" s="9">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B42" s="2">
+        <v>245</v>
+      </c>
+      <c r="D42">
+        <v>257</v>
+      </c>
+      <c r="E42">
+        <v>259</v>
+      </c>
+      <c r="F42">
+        <v>261</v>
+      </c>
+      <c r="G42" t="s">
+        <v>163</v>
+      </c>
+      <c r="H42" t="s">
+        <v>164</v>
+      </c>
+      <c r="I42" t="s">
+        <v>165</v>
+      </c>
+      <c r="K42" s="9">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="B43" s="2">
+        <v>1016</v>
+      </c>
+      <c r="D43">
+        <v>1123</v>
+      </c>
+      <c r="E43">
+        <v>1128.8</v>
+      </c>
+      <c r="F43">
+        <v>1136</v>
+      </c>
+      <c r="G43" t="s">
+        <v>167</v>
+      </c>
+      <c r="H43" t="s">
+        <v>168</v>
+      </c>
+      <c r="I43" t="s">
+        <v>169</v>
+      </c>
+      <c r="K43" s="9">
+        <f t="shared" si="0"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="B44" s="2">
+        <v>127</v>
+      </c>
+      <c r="D44">
+        <v>137</v>
+      </c>
+      <c r="E44">
+        <v>137</v>
+      </c>
+      <c r="F44">
+        <v>137</v>
+      </c>
+      <c r="G44" t="s">
+        <v>171</v>
+      </c>
+      <c r="H44" t="s">
+        <v>172</v>
+      </c>
+      <c r="I44" t="s">
+        <v>173</v>
+      </c>
+      <c r="K44" s="9">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>174</v>
+      </c>
+      <c r="B45" s="2">
         <v>155</v>
       </c>
-      <c r="H41" t="s">
-        <v>156</v>
-      </c>
-      <c r="I41" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>158</v>
-      </c>
-      <c r="D42">
-        <v>856</v>
-      </c>
-      <c r="E42">
-        <v>865.2</v>
-      </c>
-      <c r="F42">
-        <v>875</v>
-      </c>
-      <c r="G42" t="s">
-        <v>159</v>
-      </c>
-      <c r="H42" t="s">
-        <v>160</v>
-      </c>
-      <c r="I42" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="D43">
-        <v>257</v>
-      </c>
-      <c r="E43">
-        <v>259</v>
-      </c>
-      <c r="F43">
-        <v>261</v>
-      </c>
-      <c r="G43" t="s">
-        <v>163</v>
-      </c>
-      <c r="H43" t="s">
-        <v>164</v>
-      </c>
-      <c r="I43" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="D44">
-        <v>1123</v>
-      </c>
-      <c r="E44">
-        <v>1128.8</v>
-      </c>
-      <c r="F44">
-        <v>1136</v>
-      </c>
-      <c r="G44" t="s">
-        <v>167</v>
-      </c>
-      <c r="H44" t="s">
-        <v>168</v>
-      </c>
-      <c r="I44" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="10" t="s">
-        <v>170</v>
-      </c>
       <c r="D45">
-        <v>137</v>
+        <v>175</v>
       </c>
       <c r="E45">
-        <v>137</v>
+        <v>175</v>
       </c>
       <c r="F45">
-        <v>137</v>
+        <v>175</v>
       </c>
       <c r="G45" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="H45" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="I45" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+      <c r="K45" s="9">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>174</v>
+        <v>178</v>
+      </c>
+      <c r="B46" s="2">
+        <v>84</v>
       </c>
       <c r="D46">
-        <v>175</v>
+        <v>85</v>
       </c>
       <c r="E46">
-        <v>175</v>
+        <v>86.2</v>
       </c>
       <c r="F46">
-        <v>175</v>
+        <v>87</v>
       </c>
       <c r="G46" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="H46" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="I46" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+      <c r="K46" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>178</v>
+        <v>182</v>
+      </c>
+      <c r="B47" s="2">
+        <v>64</v>
       </c>
       <c r="D47">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E47">
-        <v>86.2</v>
+        <v>72</v>
       </c>
       <c r="F47">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="G47" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="H47" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="I47" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+      <c r="K47" s="9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>182</v>
+        <v>186</v>
+      </c>
+      <c r="B48" s="2">
+        <v>2018</v>
       </c>
       <c r="D48">
-        <v>72</v>
+        <v>2068</v>
       </c>
       <c r="E48">
-        <v>72</v>
+        <v>2073.6</v>
       </c>
       <c r="F48">
-        <v>72</v>
+        <v>2080</v>
       </c>
       <c r="G48" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="H48" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="I48" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>186</v>
+        <v>189</v>
+      </c>
+      <c r="K48" s="9">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="B49" s="2">
+        <v>3466</v>
       </c>
       <c r="D49">
-        <v>2068</v>
+        <v>3657</v>
       </c>
       <c r="E49">
-        <v>2073.6</v>
+        <v>3668.8</v>
       </c>
       <c r="F49">
-        <v>2080</v>
+        <v>3679</v>
       </c>
       <c r="G49" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="H49" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="I49" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="10" t="s">
-        <v>190</v>
+        <v>193</v>
+      </c>
+      <c r="K49" s="9">
+        <f t="shared" si="0"/>
+        <v>191</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="B50" s="2">
+        <v>61</v>
       </c>
       <c r="D50">
-        <v>3657</v>
+        <v>444</v>
       </c>
       <c r="E50">
-        <v>3668.8</v>
+        <v>459.6</v>
       </c>
       <c r="F50">
-        <v>3679</v>
+        <v>474</v>
       </c>
       <c r="G50" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="H50" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="I50" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="10"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>194</v>
+        <v>197</v>
+      </c>
+      <c r="K50" s="9">
+        <f t="shared" si="0"/>
+        <v>383</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="B51" s="2">
+        <v>71749</v>
+      </c>
+      <c r="D51">
+        <v>84814</v>
+      </c>
+      <c r="E51">
+        <v>85629.8</v>
+      </c>
+      <c r="F51">
+        <v>86253</v>
+      </c>
+      <c r="G51" t="s">
+        <v>199</v>
+      </c>
+      <c r="H51" t="s">
+        <v>200</v>
+      </c>
+      <c r="I51" t="s">
+        <v>201</v>
+      </c>
+      <c r="K51" s="9">
+        <f t="shared" si="0"/>
+        <v>13065</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="B52" s="2">
+        <v>41196</v>
       </c>
       <c r="D52">
-        <v>444</v>
+        <v>71241</v>
       </c>
       <c r="E52">
-        <v>459.6</v>
+        <v>73088.800000000003</v>
       </c>
       <c r="F52">
-        <v>474</v>
+        <v>74544</v>
       </c>
       <c r="G52" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="H52" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="I52" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="K52" s="9">
+        <f t="shared" si="0"/>
+        <v>30045</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
-        <v>198</v>
+        <v>206</v>
+      </c>
+      <c r="B53" s="2">
+        <v>71556</v>
       </c>
       <c r="D53">
-        <v>84814</v>
-      </c>
-      <c r="E53">
-        <v>85629.8</v>
+        <v>83161</v>
+      </c>
+      <c r="E53" s="5">
+        <v>86006</v>
       </c>
       <c r="F53">
-        <v>86253</v>
+        <v>87744</v>
       </c>
       <c r="G53" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="H53" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="I53" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+      <c r="K53" s="9">
+        <f t="shared" si="0"/>
+        <v>11605</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>202</v>
+        <v>210</v>
+      </c>
+      <c r="B54" s="2">
+        <v>109471</v>
       </c>
       <c r="D54">
-        <v>71241</v>
+        <v>134691</v>
       </c>
       <c r="E54">
-        <v>73088.800000000003</v>
+        <v>135201.79999999999</v>
       </c>
       <c r="F54">
-        <v>74544</v>
+        <v>136134</v>
       </c>
       <c r="G54" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="H54" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="I54" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+      <c r="K54" s="9">
+        <f t="shared" si="0"/>
+        <v>25220</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
-        <v>206</v>
+        <v>214</v>
+      </c>
+      <c r="B55" s="2">
+        <v>38963</v>
       </c>
       <c r="D55">
-        <v>83161</v>
-      </c>
-      <c r="E55" s="5">
-        <v>86006</v>
+        <v>147721</v>
+      </c>
+      <c r="E55">
+        <v>149248</v>
       </c>
       <c r="F55">
-        <v>87744</v>
+        <v>150392</v>
       </c>
       <c r="G55" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="H55" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I55" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="D56">
-        <v>134691</v>
-      </c>
-      <c r="E56">
-        <v>135201.79999999999</v>
-      </c>
-      <c r="F56">
-        <v>136134</v>
-      </c>
-      <c r="G56" t="s">
-        <v>211</v>
-      </c>
-      <c r="H56" t="s">
-        <v>212</v>
-      </c>
-      <c r="I56" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="D57">
-        <v>147721</v>
-      </c>
-      <c r="E57">
-        <v>149248</v>
-      </c>
-      <c r="F57">
-        <v>150392</v>
-      </c>
-      <c r="G57" t="s">
-        <v>215</v>
-      </c>
-      <c r="H57" t="s">
-        <v>216</v>
-      </c>
-      <c r="I57" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K55" s="9">
+        <f t="shared" si="0"/>
+        <v>108758</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="10"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="10"/>
+      <c r="E57" s="5"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="10"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="10"/>
-      <c r="E59" s="5"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Tabu search documentation completed
</commit_message>
<xml_diff>
--- a/hw2_GRASP/Results.xlsx
+++ b/hw2_GRASP/Results.xlsx
@@ -607,30 +607,30 @@
         <v>18230</v>
       </c>
       <c r="D5" t="n">
-        <v>20930</v>
+        <v>20705</v>
       </c>
       <c r="E5" s="15" t="n">
-        <v>21020</v>
+        <v>21005</v>
       </c>
       <c r="F5" t="n">
-        <v>21110</v>
+        <v>21230</v>
       </c>
       <c r="G5" t="n">
-        <v>90</v>
+        <v>152.7743433957417</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>3.8325</t>
+          <t>3.6313</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>3.9232</t>
+          <t>3.8834</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>4.0140</t>
+          <t>4.0394</t>
         </is>
       </c>
       <c r="L5">
@@ -651,24 +651,27 @@
         <v>2125</v>
       </c>
       <c r="E6" t="n">
-        <v>2125</v>
+        <v>2317.5</v>
       </c>
       <c r="F6" t="n">
-        <v>2125</v>
+        <v>2700</v>
+      </c>
+      <c r="G6" t="n">
+        <v>241.363315356746</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>7.9125</t>
+          <t>8.3858</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>8.2295</t>
+          <t>8.6053</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>8.5833</t>
+          <t>9.1285</t>
         </is>
       </c>
       <c r="L6">
@@ -686,29 +689,30 @@
         <v>8026</v>
       </c>
       <c r="D7" t="n">
-        <v>10741</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>11249.2</t>
-        </is>
+        <v>10800</v>
+      </c>
+      <c r="E7" t="n">
+        <v>11156.3</v>
       </c>
       <c r="F7" t="n">
-        <v>11475</v>
+        <v>11418</v>
+      </c>
+      <c r="G7" t="n">
+        <v>172.11278279082</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>1.9532</t>
+          <t>2.0405</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>2.1721</t>
+          <t>2.1065</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>2.4002</t>
+          <t>2.2325</t>
         </is>
       </c>
       <c r="L7">
@@ -726,29 +730,30 @@
         <v>40419</v>
       </c>
       <c r="D8" t="n">
-        <v>44566</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>45606.9</t>
-        </is>
+        <v>45562</v>
+      </c>
+      <c r="E8" t="n">
+        <v>45934.7</v>
       </c>
       <c r="F8" t="n">
-        <v>46400</v>
+        <v>46236</v>
+      </c>
+      <c r="G8" t="n">
+        <v>267.6920058574779</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>3.3997</t>
+          <t>3.5587</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>3.6471</t>
+          <t>3.7045</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>3.8445</t>
+          <t>3.8457</t>
         </is>
       </c>
       <c r="L8">
@@ -766,29 +771,30 @@
         <v>39420</v>
       </c>
       <c r="D9" t="n">
-        <v>48588</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>49968.0</t>
-        </is>
+        <v>49497</v>
+      </c>
+      <c r="E9" t="n">
+        <v>50450.7</v>
       </c>
       <c r="F9" t="n">
-        <v>51023</v>
+        <v>51038</v>
+      </c>
+      <c r="G9" t="n">
+        <v>463.5437519803282</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>9.2160</t>
+          <t>9.4456</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>9.4826</t>
+          <t>9.5748</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>9.6200</t>
+          <t>9.7153</t>
         </is>
       </c>
       <c r="L9">
@@ -806,29 +812,30 @@
         <v>49499</v>
       </c>
       <c r="D10" t="n">
-        <v>60161</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>63202.9</t>
-        </is>
+        <v>61789</v>
+      </c>
+      <c r="E10" t="n">
+        <v>64324.8</v>
       </c>
       <c r="F10" t="n">
-        <v>67032</v>
+        <v>65698</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1085.459423470081</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>5.9466</t>
+          <t>6.2014</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>6.2631</t>
+          <t>6.3662</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>6.6445</t>
+          <t>6.6981</t>
         </is>
       </c>
       <c r="L10">
@@ -854,19 +861,22 @@
       <c r="F11" t="n">
         <v>29120</v>
       </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>1.3682</t>
+          <t>1.4019</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1.4517</t>
+          <t>1.4627</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>1.5105</t>
+          <t>1.5016</t>
         </is>
       </c>
       <c r="L11">
@@ -892,19 +902,22 @@
       <c r="F12" t="n">
         <v>84820</v>
       </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>1.0476</t>
+          <t>0.9649</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>1.1261</t>
+          <t>1.0161</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>1.2562</t>
+          <t>1.1380</t>
         </is>
       </c>
       <c r="L12">
@@ -922,27 +935,30 @@
         <v>1123</v>
       </c>
       <c r="D13" t="n">
-        <v>2062</v>
+        <v>2222</v>
       </c>
       <c r="E13" t="n">
-        <v>2248.6</v>
+        <v>2281.4</v>
       </c>
       <c r="F13" t="n">
-        <v>2378</v>
+        <v>2383</v>
+      </c>
+      <c r="G13" t="n">
+        <v>54.19261942368167</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>7.8009</t>
+          <t>7.9459</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>8.0781</t>
+          <t>8.2255</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>8.3549</t>
+          <t>8.5848</t>
         </is>
       </c>
       <c r="L13">
@@ -968,19 +984,22 @@
       <c r="F14" t="n">
         <v>417</v>
       </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>1.2846</t>
+          <t>1.3280</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>1.3691</t>
+          <t>1.4107</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>1.5334</t>
+          <t>1.5175</t>
         </is>
       </c>
       <c r="L14">
@@ -1006,19 +1025,22 @@
       <c r="F15" t="n">
         <v>2477</v>
       </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>1.0850</t>
+          <t>1.1798</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>1.1679</t>
+          <t>1.2554</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>1.3081</t>
+          <t>1.3121</t>
         </is>
       </c>
       <c r="L15">
@@ -1036,27 +1058,30 @@
         <v>912</v>
       </c>
       <c r="D16" t="n">
-        <v>1530</v>
+        <v>1471</v>
       </c>
       <c r="E16" t="n">
-        <v>1563</v>
+        <v>1591.4</v>
       </c>
       <c r="F16" t="n">
-        <v>1623</v>
+        <v>1727</v>
+      </c>
+      <c r="G16" t="n">
+        <v>66.11232865358775</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2.6015</t>
+          <t>2.6519</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>2.7256</t>
+          <t>2.8431</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>2.9206</t>
+          <t>3.0668</t>
         </is>
       </c>
       <c r="L16">
@@ -1074,27 +1099,30 @@
         <v>915</v>
       </c>
       <c r="D17" t="n">
-        <v>1560</v>
+        <v>1496</v>
       </c>
       <c r="E17" t="n">
-        <v>1658.4</v>
+        <v>1657.2</v>
       </c>
       <c r="F17" t="n">
-        <v>1812</v>
+        <v>1720</v>
+      </c>
+      <c r="G17" t="n">
+        <v>68.26975904454329</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2.9690</t>
+          <t>3.1675</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>3.2334</t>
+          <t>3.3061</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>3.5530</t>
+          <t>3.4971</t>
         </is>
       </c>
       <c r="L17">
@@ -1112,27 +1140,30 @@
         <v>879</v>
       </c>
       <c r="D18" t="n">
-        <v>1608</v>
+        <v>1466</v>
       </c>
       <c r="E18" t="n">
-        <v>1665.2</v>
+        <v>1620.9</v>
       </c>
       <c r="F18" t="n">
-        <v>1762</v>
+        <v>1686</v>
+      </c>
+      <c r="G18" t="n">
+        <v>60.39279758381789</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>3.4080</t>
+          <t>3.6677</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>3.7098</t>
+          <t>3.8577</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>4.1187</t>
+          <t>4.0441</t>
         </is>
       </c>
       <c r="L18">
@@ -1150,27 +1181,30 @@
         <v>400</v>
       </c>
       <c r="D19" t="n">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="E19" t="n">
-        <v>475.2</v>
+        <v>474.2</v>
       </c>
       <c r="F19" t="n">
-        <v>476</v>
+        <v>478</v>
+      </c>
+      <c r="G19" t="n">
+        <v>2.481934729198171</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>1.7683</t>
+          <t>1.8221</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>1.8415</t>
+          <t>1.9523</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>1.9509</t>
+          <t>2.1566</t>
         </is>
       </c>
       <c r="L19">
@@ -1188,27 +1222,30 @@
         <v>397</v>
       </c>
       <c r="D20" t="n">
-        <v>501</v>
+        <v>486</v>
       </c>
       <c r="E20" t="n">
-        <v>507.8</v>
+        <v>505.5</v>
       </c>
       <c r="F20" t="n">
-        <v>517</v>
+        <v>515</v>
+      </c>
+      <c r="G20" t="n">
+        <v>8.891006692158093</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>1.6675</t>
+          <t>1.7554</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>1.7497</t>
+          <t>1.8873</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>1.9154</t>
+          <t>2.0016</t>
         </is>
       </c>
       <c r="L20">
@@ -1226,27 +1263,30 @@
         <v>467</v>
       </c>
       <c r="D21" t="n">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="E21" t="n">
-        <v>546.8</v>
+        <v>547</v>
       </c>
       <c r="F21" t="n">
-        <v>549</v>
+        <v>552</v>
+      </c>
+      <c r="G21" t="n">
+        <v>3.16227766016838</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>1.6695</t>
+          <t>1.7799</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>1.8106</t>
+          <t>1.8804</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>1.9277</t>
+          <t>1.9856</t>
         </is>
       </c>
       <c r="L21">
@@ -1264,27 +1304,30 @@
         <v>1023</v>
       </c>
       <c r="D22" t="n">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="E22" t="n">
-        <v>1343.2</v>
+        <v>1340.2</v>
       </c>
       <c r="F22" t="n">
-        <v>1362</v>
+        <v>1369</v>
+      </c>
+      <c r="G22" t="n">
+        <v>19.76765034089788</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>6.0060</t>
+          <t>6.2632</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>6.0823</t>
+          <t>6.5121</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>6.1843</t>
+          <t>6.6765</t>
         </is>
       </c>
       <c r="L22">
@@ -1302,27 +1345,30 @@
         <v>198</v>
       </c>
       <c r="D23" t="n">
-        <v>1323</v>
+        <v>1296</v>
       </c>
       <c r="E23" t="n">
-        <v>1336.2</v>
+        <v>1339.9</v>
       </c>
       <c r="F23" t="n">
-        <v>1352</v>
+        <v>1363</v>
+      </c>
+      <c r="G23" t="n">
+        <v>21.27651287217903</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>6.5961</t>
+          <t>6.5071</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>6.8382</t>
+          <t>6.7639</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>7.0040</t>
+          <t>7.8344</t>
         </is>
       </c>
       <c r="L23">
@@ -1340,27 +1386,30 @@
         <v>1494</v>
       </c>
       <c r="D24" t="n">
-        <v>1654</v>
+        <v>1650</v>
       </c>
       <c r="E24" t="n">
-        <v>1668.6</v>
+        <v>1669.6</v>
       </c>
       <c r="F24" t="n">
-        <v>1681</v>
+        <v>1685</v>
+      </c>
+      <c r="G24" t="n">
+        <v>11.74052809715134</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>6.6315</t>
+          <t>6.4244</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>6.8512</t>
+          <t>6.8421</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>7.0958</t>
+          <t>7.5466</t>
         </is>
       </c>
       <c r="L24">
@@ -1378,27 +1427,30 @@
         <v>1423</v>
       </c>
       <c r="D25" t="n">
-        <v>1641</v>
+        <v>1636</v>
       </c>
       <c r="E25" t="n">
-        <v>1683</v>
+        <v>1674.7</v>
       </c>
       <c r="F25" t="n">
-        <v>1699</v>
+        <v>1711</v>
+      </c>
+      <c r="G25" t="n">
+        <v>27.04459280521709</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>6.7349</t>
+          <t>6.8557</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>7.0234</t>
+          <t>7.4010</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>7.1377</t>
+          <t>8.0284</t>
         </is>
       </c>
       <c r="L25">
@@ -1416,27 +1468,30 @@
         <v>1361</v>
       </c>
       <c r="D26" t="n">
-        <v>1623</v>
+        <v>1594</v>
       </c>
       <c r="E26" t="n">
-        <v>1635.4</v>
+        <v>1617.9</v>
       </c>
       <c r="F26" t="n">
-        <v>1645</v>
+        <v>1653</v>
+      </c>
+      <c r="G26" t="n">
+        <v>18.26170857285813</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>7.8546</t>
+          <t>7.7638</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>8.1561</t>
+          <t>8.1136</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>8.5900</t>
+          <t>8.6785</t>
         </is>
       </c>
       <c r="L26">
@@ -1454,27 +1509,30 @@
         <v>1381</v>
       </c>
       <c r="D27" t="n">
-        <v>1678</v>
+        <v>1698</v>
       </c>
       <c r="E27" t="n">
-        <v>1709.2</v>
+        <v>1736.7</v>
       </c>
       <c r="F27" t="n">
-        <v>1735</v>
+        <v>1778</v>
+      </c>
+      <c r="G27" t="n">
+        <v>23.16484405300411</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>8.3840</t>
+          <t>8.4141</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>8.5852</t>
+          <t>8.5851</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>8.8323</t>
+          <t>8.7306</t>
         </is>
       </c>
       <c r="L27">
@@ -1492,27 +1550,30 @@
         <v>1765</v>
       </c>
       <c r="D28" t="n">
-        <v>2077</v>
+        <v>2042</v>
       </c>
       <c r="E28" t="n">
-        <v>2091.6</v>
+        <v>2077.8</v>
       </c>
       <c r="F28" t="n">
-        <v>2111</v>
+        <v>2107</v>
+      </c>
+      <c r="G28" t="n">
+        <v>22.1485891198514</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>12.001</t>
+          <t>10.187</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>10.228</t>
+          <t>10.328</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>9.8187</t>
+          <t>10.618</t>
         </is>
       </c>
       <c r="L28">
@@ -1530,27 +1591,30 @@
         <v>1750</v>
       </c>
       <c r="D29" t="n">
-        <v>2101</v>
+        <v>2106</v>
       </c>
       <c r="E29" t="n">
-        <v>2128.4</v>
+        <v>2137.3</v>
       </c>
       <c r="F29" t="n">
-        <v>2144</v>
+        <v>2155</v>
+      </c>
+      <c r="G29" t="n">
+        <v>15.42108945567725</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>13.088</t>
+          <t>12.909</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>13.528</t>
+          <t>13.040</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>14.159</t>
+          <t>13.116</t>
         </is>
       </c>
       <c r="L29">
@@ -1568,27 +1632,30 @@
         <v>2033</v>
       </c>
       <c r="D30" t="n">
-        <v>2461</v>
+        <v>2430</v>
       </c>
       <c r="E30" t="n">
-        <v>2488.8</v>
+        <v>2472.7</v>
       </c>
       <c r="F30" t="n">
-        <v>2501</v>
+        <v>2509</v>
+      </c>
+      <c r="G30" t="n">
+        <v>26.63850596411143</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>18.461</t>
+          <t>17.838</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>19.102</t>
+          <t>18.022</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>19.628</t>
+          <t>18.262</t>
         </is>
       </c>
       <c r="L30">
@@ -1606,27 +1673,30 @@
         <v>2241</v>
       </c>
       <c r="D31" t="n">
-        <v>2826</v>
+        <v>2803</v>
       </c>
       <c r="E31" t="n">
-        <v>2857.2</v>
+        <v>2853.9</v>
       </c>
       <c r="F31" t="n">
-        <v>2904</v>
+        <v>2906</v>
+      </c>
+      <c r="G31" t="n">
+        <v>26.44031013433844</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>21.700</t>
+          <t>21.085</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>21.946</t>
+          <t>21.645</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>22.479</t>
+          <t>22.868</t>
         </is>
       </c>
       <c r="L31">
@@ -1644,27 +1714,30 @@
         <v>2544</v>
       </c>
       <c r="D32" t="n">
-        <v>3301</v>
+        <v>3239</v>
       </c>
       <c r="E32" t="n">
-        <v>3353.8</v>
+        <v>3349.7</v>
       </c>
       <c r="F32" t="n">
-        <v>3396</v>
+        <v>3387</v>
+      </c>
+      <c r="G32" t="n">
+        <v>40.92688602862426</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>30.687</t>
+          <t>30.017</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>31.354</t>
+          <t>30.539</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>31.793</t>
+          <t>31.072</t>
         </is>
       </c>
       <c r="L32">
@@ -1682,27 +1755,30 @@
         <v>3062</v>
       </c>
       <c r="D33" t="n">
-        <v>3930</v>
+        <v>3948</v>
       </c>
       <c r="E33" t="n">
-        <v>3992.8</v>
+        <v>3982.3</v>
       </c>
       <c r="F33" t="n">
-        <v>4043</v>
+        <v>4028</v>
+      </c>
+      <c r="G33" t="n">
+        <v>25.06411777821035</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>38.060</t>
+          <t>38.174</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>38.995</t>
+          <t>39.273</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>39.407</t>
+          <t>41.673</t>
         </is>
       </c>
       <c r="L33">
@@ -1723,24 +1799,27 @@
         <v>4576</v>
       </c>
       <c r="E34" t="n">
-        <v>4617.2</v>
+        <v>4624.3</v>
       </c>
       <c r="F34" t="n">
-        <v>4674</v>
+        <v>4689</v>
+      </c>
+      <c r="G34" t="n">
+        <v>34.24047312757229</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>54.148</t>
+          <t>54.972</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>55.410</t>
+          <t>55.581</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>56.633</t>
+          <t>56.890</t>
         </is>
       </c>
       <c r="L34">
@@ -1758,27 +1837,30 @@
         <v>2568</v>
       </c>
       <c r="D35" t="n">
-        <v>4583</v>
+        <v>4608</v>
       </c>
       <c r="E35" t="n">
-        <v>4643.2</v>
+        <v>4649.1</v>
       </c>
       <c r="F35" t="n">
-        <v>4716</v>
+        <v>4711</v>
+      </c>
+      <c r="G35" t="n">
+        <v>27.72886582606653</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>100.29</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>99.833</t>
+          <t>99.219</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>99.956</t>
+          <t>99.177</t>
         </is>
       </c>
       <c r="L35">
@@ -1796,27 +1878,30 @@
         <v>2545</v>
       </c>
       <c r="D36" t="n">
-        <v>4746</v>
+        <v>4764</v>
       </c>
       <c r="E36" t="n">
-        <v>4802.6</v>
+        <v>4819</v>
       </c>
       <c r="F36" t="n">
-        <v>4859</v>
+        <v>4875</v>
+      </c>
+      <c r="G36" t="n">
+        <v>37.9130584363752</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>118.75</t>
+          <t>116.64</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>120.36</t>
+          <t>119.49</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>123.48</t>
+          <t>128.67</t>
         </is>
       </c>
       <c r="L36">
@@ -1842,19 +1927,22 @@
       <c r="F37" t="n">
         <v>20407</v>
       </c>
+      <c r="G37" t="n">
+        <v>0</v>
+      </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>1.5763</t>
+          <t>1.6712</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>1.6015</t>
+          <t>1.7893</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>1.6224</t>
+          <t>1.9008</t>
         </is>
       </c>
       <c r="L37">
@@ -1880,19 +1968,22 @@
       <c r="F38" t="n">
         <v>26118</v>
       </c>
+      <c r="G38" t="n">
+        <v>0</v>
+      </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>1.2955</t>
+          <t>1.3358</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>1.3214</t>
+          <t>1.3697</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>1.3502</t>
+          <t>1.4068</t>
         </is>
       </c>
       <c r="L38">
@@ -1910,27 +2001,30 @@
         <v>1109</v>
       </c>
       <c r="D39" t="n">
-        <v>1177</v>
+        <v>1179</v>
       </c>
       <c r="E39" t="n">
-        <v>1185</v>
+        <v>1185.4</v>
       </c>
       <c r="F39" t="n">
-        <v>1194</v>
+        <v>1195</v>
+      </c>
+      <c r="G39" t="n">
+        <v>5.023942674832188</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>4.7513</t>
+          <t>4.7573</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>4.8959</t>
+          <t>5.2368</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>5.1867</t>
+          <t>6.9856</t>
         </is>
       </c>
       <c r="L39">
@@ -1948,27 +2042,30 @@
         <v>577</v>
       </c>
       <c r="D40" t="n">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="E40" t="n">
-        <v>586.4</v>
+        <v>584.6</v>
       </c>
       <c r="F40" t="n">
-        <v>587</v>
+        <v>588</v>
+      </c>
+      <c r="G40" t="n">
+        <v>2.244994432064365</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2.1583</t>
+          <t>2.2162</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>2.2547</t>
+          <t>2.3666</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>2.4721</t>
+          <t>2.4969</t>
         </is>
       </c>
       <c r="L40">
@@ -1986,27 +2083,30 @@
         <v>791</v>
       </c>
       <c r="D41" t="n">
-        <v>856</v>
+        <v>859</v>
       </c>
       <c r="E41" t="n">
-        <v>865.2</v>
+        <v>868.7</v>
       </c>
       <c r="F41" t="n">
-        <v>875</v>
+        <v>876</v>
+      </c>
+      <c r="G41" t="n">
+        <v>5.984145720150872</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>3.9890</t>
+          <t>4.1719</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>4.0605</t>
+          <t>4.3972</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>4.1194</t>
+          <t>4.8280</t>
         </is>
       </c>
       <c r="L41">
@@ -2024,27 +2124,30 @@
         <v>245</v>
       </c>
       <c r="D42" t="n">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E42" t="n">
-        <v>259</v>
+        <v>259.6</v>
       </c>
       <c r="F42" t="n">
         <v>261</v>
       </c>
+      <c r="G42" t="n">
+        <v>2.009975124224178</v>
+      </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>1.1449</t>
+          <t>1.1660</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>1.2211</t>
+          <t>1.2501</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>1.3740</t>
+          <t>1.5185</t>
         </is>
       </c>
       <c r="L42">
@@ -2062,27 +2165,30 @@
         <v>1016</v>
       </c>
       <c r="D43" t="n">
-        <v>1123</v>
+        <v>1107</v>
       </c>
       <c r="E43" t="n">
-        <v>1128.8</v>
+        <v>1122.2</v>
       </c>
       <c r="F43" t="n">
-        <v>1136</v>
+        <v>1137</v>
+      </c>
+      <c r="G43" t="n">
+        <v>9.086253353280437</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>8.5176</t>
+          <t>8.6328</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>8.6370</t>
+          <t>9.3151</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>8.7726</t>
+          <t>9.9664</t>
         </is>
       </c>
       <c r="L43">
@@ -2108,19 +2214,22 @@
       <c r="F44" t="n">
         <v>137</v>
       </c>
+      <c r="G44" t="n">
+        <v>0</v>
+      </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>0.4084</t>
+          <t>0.4129</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>0.4323</t>
+          <t>0.4573</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>0.4775</t>
+          <t>0.5135</t>
         </is>
       </c>
       <c r="L44">
@@ -2146,19 +2255,22 @@
       <c r="F45" t="n">
         <v>175</v>
       </c>
+      <c r="G45" t="n">
+        <v>0</v>
+      </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>0.6161</t>
+          <t>0.6667</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>0.6451</t>
+          <t>0.7698</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>0.6712</t>
+          <t>1.0308</t>
         </is>
       </c>
       <c r="L45">
@@ -2176,27 +2288,30 @@
         <v>84</v>
       </c>
       <c r="D46" t="n">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E46" t="n">
-        <v>86.2</v>
+        <v>87.2</v>
       </c>
       <c r="F46" t="n">
-        <v>87</v>
+        <v>89</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0.6</v>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>1.6542</t>
+          <t>1.7124</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>1.7778</t>
+          <t>1.9181</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>1.8768</t>
+          <t>2.0517</t>
         </is>
       </c>
       <c r="L46">
@@ -2222,19 +2337,22 @@
       <c r="F47" t="n">
         <v>72</v>
       </c>
+      <c r="G47" t="n">
+        <v>0</v>
+      </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>0.3459</t>
+          <t>0.3705</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>0.3598</t>
+          <t>0.3926</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>0.3951</t>
+          <t>0.4497</t>
         </is>
       </c>
       <c r="L47">
@@ -2252,27 +2370,30 @@
         <v>2018</v>
       </c>
       <c r="D48" t="n">
-        <v>2068</v>
+        <v>2040</v>
       </c>
       <c r="E48" t="n">
-        <v>2073.6</v>
+        <v>2066.4</v>
       </c>
       <c r="F48" t="n">
-        <v>2080</v>
+        <v>2076</v>
+      </c>
+      <c r="G48" t="n">
+        <v>10.57544325312183</v>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>23.296</t>
+          <t>23.483</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>23.464</t>
+          <t>24.097</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>23.676</t>
+          <t>24.947</t>
         </is>
       </c>
       <c r="L48">
@@ -2290,27 +2411,30 @@
         <v>3466</v>
       </c>
       <c r="D49" t="n">
-        <v>3657</v>
+        <v>3662</v>
       </c>
       <c r="E49" t="n">
-        <v>3668.8</v>
+        <v>3676.6</v>
       </c>
       <c r="F49" t="n">
-        <v>3679</v>
+        <v>3695</v>
+      </c>
+      <c r="G49" t="n">
+        <v>10.73498952025571</v>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>107.35</t>
+          <t>103.70</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>107.63</t>
+          <t>105.47</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>107.94</t>
+          <t>106.88</t>
         </is>
       </c>
       <c r="L49">
@@ -2328,29 +2452,30 @@
         <v>61</v>
       </c>
       <c r="D50" t="n">
-        <v>393</v>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>448.7</t>
-        </is>
+        <v>445</v>
+      </c>
+      <c r="E50" t="n">
+        <v>465.4</v>
       </c>
       <c r="F50" t="n">
-        <v>483</v>
+        <v>482</v>
+      </c>
+      <c r="G50" t="n">
+        <v>11.84229707446997</v>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>56.464</t>
+          <t>52.083</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>56.704</t>
+          <t>53.056</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>56.955</t>
+          <t>55.935</t>
         </is>
       </c>
       <c r="L50">
@@ -2368,27 +2493,30 @@
         <v>71749</v>
       </c>
       <c r="D51" t="n">
-        <v>84814</v>
+        <v>84136</v>
       </c>
       <c r="E51" t="n">
-        <v>85629.8</v>
+        <v>84921.60000000001</v>
       </c>
       <c r="F51" t="n">
-        <v>86253</v>
+        <v>85695</v>
+      </c>
+      <c r="G51" t="n">
+        <v>506.5979076151026</v>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>24.674</t>
+          <t>24.117</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>25.005</t>
+          <t>24.379</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>25.163</t>
+          <t>24.599</t>
         </is>
       </c>
       <c r="L51">
@@ -2406,27 +2534,30 @@
         <v>41196</v>
       </c>
       <c r="D52" t="n">
-        <v>71241</v>
+        <v>70393</v>
       </c>
       <c r="E52" t="n">
-        <v>73088.8</v>
+        <v>72281.60000000001</v>
       </c>
       <c r="F52" t="n">
-        <v>74544</v>
+        <v>73968</v>
+      </c>
+      <c r="G52" t="n">
+        <v>1335.389171739834</v>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>19.661</t>
+          <t>19.261</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>19.811</t>
+          <t>19.426</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>20.100</t>
+          <t>19.664</t>
         </is>
       </c>
       <c r="L52">
@@ -2444,27 +2575,30 @@
         <v>71556</v>
       </c>
       <c r="D53" t="n">
-        <v>83161</v>
+        <v>85324</v>
       </c>
       <c r="E53" t="n">
-        <v>86006</v>
+        <v>86406.60000000001</v>
       </c>
       <c r="F53" t="n">
-        <v>87744</v>
+        <v>87442</v>
+      </c>
+      <c r="G53" t="n">
+        <v>841.8138986735727</v>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>24.430</t>
+          <t>24.086</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>24.736</t>
+          <t>24.398</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>24.873</t>
+          <t>24.673</t>
         </is>
       </c>
       <c r="L53">
@@ -2482,27 +2616,30 @@
         <v>109471</v>
       </c>
       <c r="D54" t="n">
-        <v>134691</v>
+        <v>134722</v>
       </c>
       <c r="E54" t="n">
-        <v>135201.8</v>
+        <v>135044.6</v>
       </c>
       <c r="F54" t="n">
-        <v>136134</v>
+        <v>135623</v>
+      </c>
+      <c r="G54" t="n">
+        <v>329.8039417593428</v>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>72.406</t>
+          <t>69.783</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>72.763</t>
+          <t>70.259</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>73.572</t>
+          <t>71.458</t>
         </is>
       </c>
       <c r="L54">
@@ -2520,29 +2657,30 @@
         <v>38963</v>
       </c>
       <c r="D55" t="n">
-        <v>144545</v>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>148052.9</t>
-        </is>
+        <v>144979</v>
+      </c>
+      <c r="E55" t="n">
+        <v>148138.2</v>
       </c>
       <c r="F55" t="n">
-        <v>150760</v>
+        <v>150839</v>
+      </c>
+      <c r="G55" t="n">
+        <v>2332.633310231164</v>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>120.11</t>
+          <t>115.04</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>120.86</t>
+          <t>119.67</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>121.68</t>
+          <t>122.12</t>
         </is>
       </c>
       <c r="L55">

</xml_diff>